<commit_message>
fixed fixation dot position
</commit_message>
<xml_diff>
--- a/stimuli_en/multipleye-other-screens-en.xlsx
+++ b/stimuli_en/multipleye-other-screens-en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-image-creation/stimuli_en/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA4DCCF-5756-DF47-8C36-559E8A608C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A9EF16-76B4-594F-A787-CF657A88DE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{367FC362-8E62-214D-8B47-8D2B5F85E7DC}"/>
   </bookViews>
@@ -102,9 +102,6 @@
     <t>We will start with two additional practice texts now so that you know how the experiment works.</t>
   </si>
   <si>
-    <t>This is the end of the practice part. If you are ready, we will start with the experiment. Please try to move as little as possible while reading the texts in order to avoid re-calibrations of the eye-tracker.</t>
-  </si>
-  <si>
     <t>Right before practice stimuli</t>
   </si>
   <si>
@@ -118,9 +115,13 @@
 The experimenter will ask you to do so now. </t>
   </si>
   <si>
+    <t>This is the end of the practice part. If you are ready, we will start with the experiment. Please try to move as little as possible while reading the texts in order to avoid re-calibrations of the eye-tracker.
+Please press space if you are ready.</t>
+  </si>
+  <si>
     <t>In this experiment you will read a series of texts of differing length. Each text is divided into multiple pages (screens). Please read the text as you would read any other text. When you are finished with one page, look at the bottom right corner of the screen and press the **space bar.** Then the next page will appear. After each text you will have to answer a few multiple choice questions about the text. You can use the keyboard to pick an answer. **You won't be able to go back to a page or a question you have already read.**
-Right before each new text screen there is a fixation dot shown at the top left corner of the screen. The next page will only appear if you steadily look at the dot.
-In between two texts there might be a re-calibration.</t>
+Right before each new text screen there is a fixation dot shown at the top left corner of the screen. The next page will only appear if you steadily look at the dot. In between two texts there might be a re-calibration.
+Please press space if you are ready.</t>
   </si>
 </sst>
 </file>
@@ -478,7 +479,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,7 +566,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="238" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="255" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -590,10 +591,10 @@
         <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -601,7 +602,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>19</v>
@@ -612,13 +613,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>